<commit_message>
Fix for combined chart axis ids.
</commit_message>
<xml_diff>
--- a/xlsxwriter/test/comparison/xlsx_files/chart_combined02.xlsx
+++ b/xlsxwriter/test/comparison/xlsx_files/chart_combined02.xlsx
@@ -92,8 +92,8 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="84882560"/>
-        <c:axId val="84884096"/>
+        <c:axId val="50010001"/>
+        <c:axId val="50010002"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -129,24 +129,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="84882560"/>
-        <c:axId val="84884096"/>
+        <c:axId val="50010001"/>
+        <c:axId val="50010002"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84882560"/>
+        <c:axId val="50010001"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84884096"/>
+        <c:crossAx val="50010002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84884096"/>
+        <c:axId val="50010002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -154,7 +154,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84882560"/>
+        <c:crossAx val="50010001"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>